<commit_message>
Add tests on _make_route
</commit_message>
<xml_diff>
--- a/tests/test_data/fwt_case6.xlsx
+++ b/tests/test_data/fwt_case6.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{F390F16B-2CCF-41A4-B1CF-58362352A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67E02F6F-2D37-4AC6-8E9E-F80BB53D5C6D}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{F390F16B-2CCF-41A4-B1CF-58362352A2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0EA0205-5236-41A4-BDD1-3643223D9A7A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C2FBD1F4-2459-45CD-802C-891B8518D02E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C2FBD1F4-2459-45CD-802C-891B8518D02E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>-2</t>
   </si>
   <si>
-    <t>0000000000</t>
-  </si>
-  <si>
     <t>FERT</t>
   </si>
   <si>
@@ -90,40 +87,49 @@
     <t>Standard Price</t>
   </si>
   <si>
-    <t>2100</t>
-  </si>
-  <si>
-    <t>FR</t>
-  </si>
-  <si>
-    <t>8122500840</t>
-  </si>
-  <si>
-    <t>701</t>
-  </si>
-  <si>
-    <t>00001</t>
-  </si>
-  <si>
-    <t>Echo</t>
-  </si>
-  <si>
-    <t>Echo 15</t>
-  </si>
-  <si>
-    <t>C346904</t>
-  </si>
-  <si>
-    <t>2001CZD4079</t>
-  </si>
-  <si>
-    <t>8122502140</t>
-  </si>
-  <si>
-    <t>702</t>
-  </si>
-  <si>
-    <t>2001CZ00NEW</t>
+    <t>K</t>
+  </si>
+  <si>
+    <t>632</t>
+  </si>
+  <si>
+    <t>2200</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>8123730680</t>
+  </si>
+  <si>
+    <t>00296</t>
+  </si>
+  <si>
+    <t>0000385977</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Charlie 22</t>
+  </si>
+  <si>
+    <t>I638176</t>
+  </si>
+  <si>
+    <t>2305PXT6252</t>
+  </si>
+  <si>
+    <t>9000667710</t>
+  </si>
+  <si>
+    <t>8123731130</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>0000007905</t>
   </si>
 </sst>
 </file>
@@ -502,159 +508,207 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F80F7D-A43A-4668-8C29-D1C2FA45569A}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>44931</v>
+        <v>44950</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H2" t="s">
         <v>23</v>
       </c>
       <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
-        <v>2</v>
-      </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>769.12</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>44931</v>
+        <v>44950</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
         <v>23</v>
       </c>
       <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" t="s">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O3">
         <v>-1</v>
       </c>
       <c r="P3">
+        <v>769.12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>44950</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
         <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4">
+        <v>-1</v>
+      </c>
+      <c r="P4">
+        <v>769.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>